<commit_message>
update data call templates
</commit_message>
<xml_diff>
--- a/data/datacall_template/00template/Eel_Data_Call_2022_Annex4_Landings_Commercial.xlsx
+++ b/data/datacall_template/00template/Eel_Data_Call_2022_Annex4_Landings_Commercial.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="24330" windowHeight="14370"/>
   </bookViews>
   <sheets>
     <sheet name="readme" sheetId="1" r:id="rId1"/>
@@ -13,7 +13,7 @@
     <sheet name="existing_discarded" sheetId="4" r:id="rId4"/>
     <sheet name="new_data" sheetId="5" r:id="rId5"/>
     <sheet name="updated_data" sheetId="6" r:id="rId6"/>
-    <sheet name="deleted_data " sheetId="7" r:id="rId7"/>
+    <sheet name="deleted_data" sheetId="7" r:id="rId7"/>
     <sheet name="tr_typeseries_ser" sheetId="8" r:id="rId8"/>
     <sheet name="tr_emu_em" sheetId="9" r:id="rId9"/>
     <sheet name="tr_country_cou" sheetId="10" r:id="rId10"/>
@@ -24,7 +24,7 @@
     <sheet name="missing values" sheetId="15" r:id="rId15"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'deleted_data '!$B$1:$K$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">deleted_data!$B$1:$K$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">existing_discarded!$A$1:$P$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">existing_kept!$A$1:$P$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">updated_data!$B$1:$K$1</definedName>
@@ -32,7 +32,7 @@
     <definedName name="data">#REF!</definedName>
     <definedName name="metadata">metadata!$B$6:$C$8</definedName>
   </definedNames>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -2740,6 +2740,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -2761,7 +2764,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="ZoneTexte 1"/>
+        <xdr:cNvPr id="2" name="ZoneTexte 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr bwMode="auto">
@@ -2894,7 +2903,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="ZoneTexte 1"/>
+        <xdr:cNvPr id="2" name="ZoneTexte 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr bwMode="auto">
@@ -2984,7 +2999,13 @@
     <xdr:ext cx="5928360" cy="4914679"/>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="ZoneTexte 1"/>
+        <xdr:cNvPr id="2" name="ZoneTexte 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0400-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr bwMode="auto">
@@ -3205,7 +3226,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Image 2"/>
+        <xdr:cNvPr id="3" name="Image 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0400-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -3242,7 +3269,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Picture 2"/>
+        <xdr:cNvPr id="4" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0400-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -3284,7 +3317,13 @@
     <xdr:ext cx="5928360" cy="1470146"/>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="ZoneTexte 1"/>
+        <xdr:cNvPr id="2" name="ZoneTexte 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr bwMode="auto">
@@ -3512,7 +3551,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Image 2"/>
+        <xdr:cNvPr id="3" name="Image 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -3549,7 +3594,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Picture 2"/>
+        <xdr:cNvPr id="4" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -3591,7 +3642,13 @@
     <xdr:ext cx="5928360" cy="1125693"/>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="ZoneTexte 1"/>
+        <xdr:cNvPr id="2" name="ZoneTexte 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0600-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr bwMode="auto">
@@ -3772,7 +3829,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Image 1"/>
+        <xdr:cNvPr id="2" name="Image 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0800-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -3813,7 +3876,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Image 1"/>
+        <xdr:cNvPr id="2" name="Image 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0900-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -3854,7 +3923,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0C00-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4095,7 +4170,7 @@
   <dimension ref="A1:B36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -9676,8 +9751,8 @@
   </sheetPr>
   <dimension ref="A1:L999"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="M48" sqref="M48"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -23693,12 +23768,32 @@
       <c r="L999" s="21"/>
     </row>
   </sheetData>
-  <dataValidations count="1">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A1:XFD1048576"/>
+  <dataValidations count="3">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1:XFD1048576"/>
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1:B1048576">
+      <formula1>0</formula1>
+      <formula2>2150</formula2>
+    </dataValidation>
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C1:C1048576">
+      <formula1>0</formula1>
+      <formula2>9.99999999999999E+42</formula2>
+    </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" firstPageNumber="4294967295" orientation="portrait"/>
   <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>tr_typeseries_ser!$B$5</xm:f>
+          </x14:formula1>
+          <xm:sqref>A1:A1048576</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -38744,8 +38839,8 @@
   </sheetPr>
   <dimension ref="A1:M999"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J22" sqref="J22"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="I47" sqref="I47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -55859,27 +55954,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="4d5313c0-c1e6-4122-afa9-da1ccdba405d"/>
-    <TaxCatchAllLabel xmlns="4d5313c0-c1e6-4122-afa9-da1ccdba405d"/>
-    <TaxKeywordTaxHTField xmlns="4d5313c0-c1e6-4122-afa9-da1ccdba405d">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </TaxKeywordTaxHTField>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010065CE7316361DFA48AC876C6112A59FE5" ma:contentTypeVersion="0" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="fb125599c9f9a751b726b9a94d2e235b">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="4d5313c0-c1e6-4122-afa9-da1ccdba405d" xmlns:ns3="362c980f-4e38-4cca-bd06-5104ee5993c5" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b91c66d6a628c7b1a21e6c64315cfea9" ns2:_="" ns3:_="">
     <xsd:import namespace="4d5313c0-c1e6-4122-afa9-da1ccdba405d"/>
@@ -56056,32 +56130,28 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{97A60C9D-8C24-4385-8428-5CB16A00628A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="4d5313c0-c1e6-4122-afa9-da1ccdba405d"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="362c980f-4e38-4cca-bd06-5104ee5993c5"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F0510A9C-5558-41DA-ACE7-0281B3CA4B88}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="4d5313c0-c1e6-4122-afa9-da1ccdba405d"/>
+    <TaxCatchAllLabel xmlns="4d5313c0-c1e6-4122-afa9-da1ccdba405d"/>
+    <TaxKeywordTaxHTField xmlns="4d5313c0-c1e6-4122-afa9-da1ccdba405d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </TaxKeywordTaxHTField>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{11819C49-9EBF-42F8-8A99-4135FBDC43AF}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -56098,4 +56168,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F0510A9C-5558-41DA-ACE7-0281B3CA4B88}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{97A60C9D-8C24-4385-8428-5CB16A00628A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="4d5313c0-c1e6-4122-afa9-da1ccdba405d"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="362c980f-4e38-4cca-bd06-5104ee5993c5"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>